<commit_message>
Solicitudes de 09_01 y correcciones de 09_02
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/SolicitudGrafica_CN_08_01_CO_REC310.xlsx
+++ b/fuentes/contenidos/grado08/guion01/SolicitudGrafica_CN_08_01_CO_REC310.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos E\Aula Planeta\Edición\Amanda Varela\CN_08_01_CO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="170">
   <si>
     <t>Fecha:</t>
   </si>
@@ -529,12 +534,6 @@
     <t>Esta imagen hace parte del recurso "Evaluación" del guion ubicado en 3° ESO/Biología y geología/La coordinación: sistema nervioso y endocrino</t>
   </si>
   <si>
-    <t>Hombre tomándose la cabeza con fuerza, con las manos</t>
-  </si>
-  <si>
-    <t>3° ESO/Biología y geología/La coordinación: sistema nervioso y endocrino/Evaluación/Hombre tomándose la cabeza con fuerza, con las manos</t>
-  </si>
-  <si>
     <t>3° ESO/Biología y geología/La coordinación: sistema nervioso y endocrino/Evaluación/Vista lateral de un cerebro</t>
   </si>
   <si>
@@ -547,9 +546,6 @@
     <t>Imagen de una sinapsis (estructuras azules, una de ellas iluminadas en amarillo)</t>
   </si>
   <si>
-    <t>3° ESO/Biología y geología/La coordinación: sistema nervioso y endocrino/Evaluación/Persona en traslúcido de color fucsia y en donde se ve el cerebro y los nervios</t>
-  </si>
-  <si>
     <t>Persona en traslúcido de color fucsia y en donde se ve el cerebro y los nervios</t>
   </si>
   <si>
@@ -569,6 +565,24 @@
   </si>
   <si>
     <t>Cerebro, médula espinal y nervios sobre fondo blanco</t>
+  </si>
+  <si>
+    <t>3° ESO/Biología y geología/La coordinación: sistema nervioso y endocrino/Evaluación/ Persona en traslúcido de color fucsia y en donde se ve el cerebro y los nervios</t>
+  </si>
+  <si>
+    <t>Esta imagen hace parte del recurso "Evaluación" del guion ubicado en 3° ESO/Biología y geología/La coordinación: docrino</t>
+  </si>
+  <si>
+    <t>Fotografía de neurona y células gliales en fondo azul</t>
+  </si>
+  <si>
+    <t>Neurona motora y músculo</t>
+  </si>
+  <si>
+    <t>Beirponas café en fondo gris</t>
+  </si>
+  <si>
+    <t>IMG10</t>
   </si>
 </sst>
 </file>
@@ -1496,6 +1510,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1580,10 +1598,6 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1743,7 +1757,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1751,6 +1765,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1784,7 +1812,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1792,6 +1820,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1825,7 +1867,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1833,6 +1875,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1866,7 +1922,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1874,6 +1930,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1907,7 +1977,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1915,6 +1985,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1948,7 +2032,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1956,6 +2040,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1989,7 +2087,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1997,6 +2095,20 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2332,9 +2444,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2372,14 +2484,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="F2" s="80" t="s">
+      <c r="D2" s="90"/>
+      <c r="F2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="81"/>
+      <c r="G2" s="83"/>
       <c r="H2" s="55"/>
       <c r="I2" s="55"/>
       <c r="J2" s="16"/>
@@ -2389,14 +2501,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="89">
+      <c r="C3" s="91">
         <v>8</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="F3" s="82">
+      <c r="D3" s="92"/>
+      <c r="F3" s="84">
         <v>42212</v>
       </c>
-      <c r="G3" s="83"/>
+      <c r="G3" s="85"/>
       <c r="H3" s="55"/>
       <c r="I3" s="55"/>
       <c r="J3" s="16"/>
@@ -2406,10 +2518,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="5"/>
       <c r="F4" s="54" t="s">
         <v>55</v>
@@ -2427,10 +2539,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="93" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="92"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="5"/>
       <c r="F5" s="52" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2481,12 +2593,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="86"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="88"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2535,7 +2647,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="80" t="s">
         <v>150</v>
       </c>
       <c r="C10" s="27" t="str">
@@ -2564,7 +2676,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J10" s="112" t="s">
+      <c r="J10" s="81" t="s">
         <v>151</v>
       </c>
       <c r="K10" s="19" t="s">
@@ -2576,8 +2688,8 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="111" t="s">
-        <v>154</v>
+      <c r="B11" s="80" t="s">
+        <v>164</v>
       </c>
       <c r="C11" s="27" t="str">
         <f t="shared" ref="C11:C22" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -2605,8 +2717,8 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J11" s="112" t="s">
-        <v>153</v>
+      <c r="J11" s="81" t="s">
+        <v>157</v>
       </c>
       <c r="K11" s="19" t="s">
         <v>152</v>
@@ -2617,8 +2729,8 @@
         <f t="shared" ref="A12:A30" si="3">IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),CONCATENATE(LEFT(A11,3),IF(MID(A11,4,2)+1&lt;10,CONCATENATE("0",MID(A11,4,2)+1))),"")</f>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="111" t="s">
-        <v>155</v>
+      <c r="B12" s="80" t="s">
+        <v>153</v>
       </c>
       <c r="C12" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2646,8 +2758,8 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J12" s="112" t="s">
-        <v>156</v>
+      <c r="J12" s="81" t="s">
+        <v>154</v>
       </c>
       <c r="K12" s="19" t="s">
         <v>152</v>
@@ -2658,8 +2770,8 @@
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="111" t="s">
-        <v>157</v>
+      <c r="B13" s="80" t="s">
+        <v>155</v>
       </c>
       <c r="C13" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2687,20 +2799,20 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J13" s="112" t="s">
-        <v>158</v>
+      <c r="J13" s="81" t="s">
+        <v>156</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
       </c>
-      <c r="B14" s="111" t="s">
-        <v>159</v>
+      <c r="B14" s="80">
+        <v>79216378</v>
       </c>
       <c r="C14" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2728,20 +2840,18 @@
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J14" s="112" t="s">
-        <v>160</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>152</v>
-      </c>
+      <c r="J14" s="81" t="s">
+        <v>166</v>
+      </c>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
-      <c r="B15" s="111" t="s">
-        <v>161</v>
+      <c r="B15" s="80" t="s">
+        <v>158</v>
       </c>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2770,7 +2880,7 @@
         <v>500 x 500 px</v>
       </c>
       <c r="J15" s="79" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K15" s="19"/>
     </row>
@@ -2779,15 +2889,19 @@
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
-      <c r="B16" s="111" t="s">
-        <v>164</v>
+      <c r="B16" s="80" t="s">
+        <v>161</v>
       </c>
       <c r="C16" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="1"/>
         <v>CN_08_01_CO_REC290_IMG07n.png</v>
@@ -2805,7 +2919,7 @@
         <v>500 x 500 px</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K16" s="36"/>
     </row>
@@ -2814,15 +2928,19 @@
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
-      <c r="B17" s="111" t="s">
-        <v>165</v>
+      <c r="B17" s="80" t="s">
+        <v>162</v>
       </c>
       <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Recurso M5A</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="F17" s="14" t="str">
         <f t="shared" si="1"/>
         <v>CN_08_01_CO_REC290_IMG08n.png</v>
@@ -2839,71 +2957,88 @@
         <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>500 x 500 px</v>
       </c>
-      <c r="J17" s="112" t="s">
-        <v>166</v>
-      </c>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="81" t="s">
+        <v>163</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B18" s="28"/>
+        <v>IMG09</v>
+      </c>
+      <c r="B18" s="28">
+        <v>311314832</v>
+      </c>
       <c r="C18" s="27" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+        <v>Recurso M5A</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>CN_08_01_CO_REC290_IMG09n.png</v>
       </c>
       <c r="G18" s="14" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>286 x 286 px</v>
       </c>
       <c r="H18" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>CN_08_01_CO_REC290_IMG09a.png</v>
       </c>
       <c r="I18" s="14" t="str">
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J18" s="21"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>167</v>
+      </c>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="34">
+        <v>285141302</v>
+      </c>
       <c r="C19" s="27" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+        <v>Recurso M5A</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="F19" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>CN_08_01_CO_REC290_IMG10n.png</v>
       </c>
       <c r="G19" s="14" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
+        <v>286 x 286 px</v>
       </c>
       <c r="H19" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>CN_08_01_CO_REC290_IMG10a.png</v>
       </c>
       <c r="I19" s="14" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J19" s="33"/>
+        <v>500 x 500 px</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>168</v>
+      </c>
       <c r="K19" s="36"/>
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -5251,25 +5386,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="97"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="46"/>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="99"/>
-      <c r="E2" s="100"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="102"/>
       <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -5277,11 +5412,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="46"/>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="106"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108"/>
       <c r="F3" s="47"/>
       <c r="H3" s="37" t="s">
         <v>18</v>
@@ -5332,11 +5467,11 @@
       <c r="C5" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="107" t="str">
+      <c r="D5" s="109" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="108"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="47"/>
       <c r="H5" s="37" t="s">
         <v>22</v>
@@ -5381,12 +5516,12 @@
       <c r="C7" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="93" t="str">
+      <c r="D7" s="95" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="93"/>
-      <c r="F7" s="94"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="96"/>
       <c r="H7" s="37" t="s">
         <v>24</v>
       </c>
@@ -5480,14 +5615,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="97"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="99"/>
       <c r="I13" s="37" t="s">
         <v>33</v>
       </c>
@@ -5520,12 +5655,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="46"/>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
-      <c r="F15" s="100"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="102"/>
       <c r="J15" s="37">
         <v>12</v>
       </c>
@@ -5565,12 +5700,12 @@
       <c r="C17" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="101" t="str">
+      <c r="D17" s="103" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="102"/>
-      <c r="F17" s="103"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="105"/>
       <c r="J17" s="37">
         <v>14</v>
       </c>
@@ -5586,12 +5721,12 @@
       <c r="C18" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="93" t="str">
+      <c r="D18" s="95" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="93"/>
-      <c r="F18" s="94"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="96"/>
       <c r="J18" s="37">
         <v>15</v>
       </c>
@@ -5983,41 +6118,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="109" t="s">
+      <c r="B1" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="109" t="s">
+      <c r="D1" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="109" t="s">
+      <c r="E1" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="109" t="s">
+      <c r="F1" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="109" t="s">
+      <c r="G1" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="110" t="s">
+      <c r="H1" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="109"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
       <c r="H2" s="56" t="s">
         <v>65</v>
       </c>

</xml_diff>